<commit_message>
status in search results
</commit_message>
<xml_diff>
--- a/data/Platelet Donors File.xlsx
+++ b/data/Platelet Donors File.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="397">
   <si>
     <t>Residence Address/Pincode</t>
   </si>
@@ -1174,6 +1174,39 @@
   </si>
   <si>
     <t>14b,flat no 410,majas wadi mandar chs,mumbai</t>
+  </si>
+  <si>
+    <t>92701 51259</t>
+  </si>
+  <si>
+    <t>98201 95179</t>
+  </si>
+  <si>
+    <t>98927 40103</t>
+  </si>
+  <si>
+    <t>98193 50700</t>
+  </si>
+  <si>
+    <t>98218 80004</t>
+  </si>
+  <si>
+    <t>98202 56689</t>
+  </si>
+  <si>
+    <t>98190 22659</t>
+  </si>
+  <si>
+    <t>98700 53982</t>
+  </si>
+  <si>
+    <t>98200 44846</t>
+  </si>
+  <si>
+    <t>93242 04541</t>
+  </si>
+  <si>
+    <t>9867 30173</t>
   </si>
 </sst>
 </file>
@@ -1181,9 +1214,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1198,6 +1231,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1417,10 +1457,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1509,14 +1553,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1822,7 +1879,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6:F162"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,7 +1931,7 @@
         <v>179</v>
       </c>
       <c r="D2" s="26">
-        <v>9820089688</v>
+        <v>9819104080</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>241</v>
@@ -1899,8 +1956,8 @@
       <c r="C3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="26">
-        <v>9820089688</v>
+      <c r="D3" s="1">
+        <v>9970531548</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>242</v>
@@ -1925,8 +1982,8 @@
       <c r="C4" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="26">
-        <v>9820089688</v>
+      <c r="D4" s="6">
+        <v>9370282922</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>243</v>
@@ -1951,8 +2008,8 @@
       <c r="C5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="26">
-        <v>9820089688</v>
+      <c r="D5" s="48">
+        <v>8425915239</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>244</v>
@@ -1977,8 +2034,8 @@
       <c r="C6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="26">
-        <v>9820089688</v>
+      <c r="D6" s="6">
+        <v>9821825967</v>
       </c>
       <c r="E6" s="34" t="s">
         <v>233</v>
@@ -2003,8 +2060,8 @@
       <c r="C7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="26">
-        <v>9820089688</v>
+      <c r="D7" s="1">
+        <v>7506367497</v>
       </c>
       <c r="E7" s="34" t="s">
         <v>245</v>
@@ -2029,8 +2086,8 @@
       <c r="C8" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="26">
-        <v>9820089688</v>
+      <c r="D8" s="6">
+        <v>9833727879</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>246</v>
@@ -2055,8 +2112,8 @@
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="26">
-        <v>9820089688</v>
+      <c r="D9" s="6">
+        <v>9029129864</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>234</v>
@@ -2079,8 +2136,8 @@
       <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="26">
-        <v>9820089688</v>
+      <c r="D10" s="6">
+        <v>9930139876</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>247</v>
@@ -2105,8 +2162,8 @@
       <c r="C11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="26">
-        <v>9820089688</v>
+      <c r="D11" s="1">
+        <v>9819295163</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>248</v>
@@ -2129,8 +2186,8 @@
       <c r="C12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="26">
-        <v>9820089688</v>
+      <c r="D12" s="6" t="s">
+        <v>386</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>249</v>
@@ -2155,8 +2212,8 @@
       <c r="C13" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="26">
-        <v>9820089688</v>
+      <c r="D13" s="1" t="s">
+        <v>387</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>250</v>
@@ -2181,8 +2238,8 @@
       <c r="C14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="26">
-        <v>9820089688</v>
+      <c r="D14" s="1">
+        <v>9820529106</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>235</v>
@@ -2207,8 +2264,8 @@
       <c r="C15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="26">
-        <v>9820089688</v>
+      <c r="D15" s="1">
+        <v>7738667165</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>251</v>
@@ -2233,8 +2290,8 @@
       <c r="C16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="26">
-        <v>9820089688</v>
+      <c r="D16" s="6">
+        <v>9004082787</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>236</v>
@@ -2259,8 +2316,8 @@
       <c r="C17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="26">
-        <v>9820089688</v>
+      <c r="D17" s="48">
+        <v>9819838994</v>
       </c>
       <c r="E17" s="34" t="s">
         <v>252</v>
@@ -2285,8 +2342,8 @@
       <c r="C18" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="26">
-        <v>9820089688</v>
+      <c r="D18" s="1">
+        <v>7767052854</v>
       </c>
       <c r="E18" s="34" t="s">
         <v>253</v>
@@ -2311,8 +2368,8 @@
       <c r="C19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="26">
-        <v>9820089688</v>
+      <c r="D19" s="1">
+        <v>9920701019</v>
       </c>
       <c r="E19" s="34" t="s">
         <v>254</v>
@@ -2335,8 +2392,8 @@
       <c r="C20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="26">
-        <v>9820089688</v>
+      <c r="D20" s="1">
+        <v>9819285335</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>255</v>
@@ -2359,8 +2416,8 @@
       <c r="C21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="26">
-        <v>9820089688</v>
+      <c r="D21" s="6">
+        <v>9821830331</v>
       </c>
       <c r="E21" s="35" t="s">
         <v>256</v>
@@ -2383,8 +2440,8 @@
       <c r="C22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="26">
-        <v>9820089688</v>
+      <c r="D22" s="1">
+        <v>9833887940</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>257</v>
@@ -2409,8 +2466,8 @@
       <c r="C23" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="26">
-        <v>9820089688</v>
+      <c r="D23" s="1">
+        <v>9833585877</v>
       </c>
       <c r="E23" s="34" t="s">
         <v>237</v>
@@ -2433,8 +2490,8 @@
       <c r="C24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="26">
-        <v>9820089688</v>
+      <c r="D24" s="6">
+        <v>9870575248</v>
       </c>
       <c r="E24" s="34" t="s">
         <v>258</v>
@@ -2459,8 +2516,8 @@
       <c r="C25" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="26">
-        <v>9820089688</v>
+      <c r="D25" s="6">
+        <v>9820410040</v>
       </c>
       <c r="E25" s="34" t="s">
         <v>259</v>
@@ -2483,8 +2540,8 @@
       <c r="C26" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="26">
-        <v>9820089688</v>
+      <c r="D26" s="6">
+        <v>9619519667</v>
       </c>
       <c r="E26" s="34" t="s">
         <v>260</v>
@@ -2509,8 +2566,8 @@
       <c r="C27" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D27" s="26">
-        <v>9820089688</v>
+      <c r="D27" s="1">
+        <v>9821309327</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>261</v>
@@ -2533,8 +2590,8 @@
       <c r="C28" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D28" s="26">
-        <v>9820089688</v>
+      <c r="D28" s="1">
+        <v>8655658667</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>262</v>
@@ -2559,8 +2616,8 @@
       <c r="C29" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="26">
-        <v>9820089688</v>
+      <c r="D29" s="6">
+        <v>9004666322</v>
       </c>
       <c r="E29" s="34" t="s">
         <v>263</v>
@@ -2585,8 +2642,8 @@
       <c r="C30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="26">
-        <v>9820089688</v>
+      <c r="D30" s="1">
+        <v>9930865658</v>
       </c>
       <c r="E30" s="34" t="s">
         <v>264</v>
@@ -2611,8 +2668,8 @@
       <c r="C31" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="26">
-        <v>9820089688</v>
+      <c r="D31" s="6" t="s">
+        <v>388</v>
       </c>
       <c r="E31" s="34" t="s">
         <v>265</v>
@@ -2637,8 +2694,8 @@
       <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="26">
-        <v>9820089688</v>
+      <c r="D32" s="49">
+        <v>9370562378</v>
       </c>
       <c r="E32" s="34" t="s">
         <v>266</v>
@@ -2663,8 +2720,8 @@
       <c r="C33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="26">
-        <v>9820089688</v>
+      <c r="D33" s="1">
+        <v>8108087091</v>
       </c>
       <c r="E33" s="34" t="s">
         <v>267</v>
@@ -2689,8 +2746,8 @@
       <c r="C34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="26">
-        <v>9820089688</v>
+      <c r="D34" s="6">
+        <v>9029879990</v>
       </c>
       <c r="E34" s="34" t="s">
         <v>268</v>
@@ -2713,8 +2770,8 @@
       <c r="C35" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="26">
-        <v>9820089688</v>
+      <c r="D35" s="6">
+        <v>9967215225</v>
       </c>
       <c r="E35" s="34" t="s">
         <v>269</v>
@@ -2739,8 +2796,8 @@
       <c r="C36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="26">
-        <v>9820089688</v>
+      <c r="D36" s="1">
+        <v>9820154551</v>
       </c>
       <c r="E36" s="34" t="s">
         <v>270</v>
@@ -2765,8 +2822,8 @@
       <c r="C37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="26">
-        <v>9820089688</v>
+      <c r="D37" s="6">
+        <v>9619922070</v>
       </c>
       <c r="E37" s="34" t="s">
         <v>271</v>
@@ -2789,8 +2846,8 @@
       <c r="C38" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D38" s="26">
-        <v>9820089688</v>
+      <c r="D38" s="1">
+        <v>8108284437</v>
       </c>
       <c r="E38" s="34" t="s">
         <v>238</v>
@@ -2813,8 +2870,8 @@
       <c r="C39" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="26">
-        <v>9820089688</v>
+      <c r="D39" s="1">
+        <v>8450984546</v>
       </c>
       <c r="E39" s="34" t="s">
         <v>272</v>
@@ -2837,8 +2894,8 @@
       <c r="C40" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="26">
-        <v>9820089688</v>
+      <c r="D40" s="1">
+        <v>9029290850</v>
       </c>
       <c r="E40" s="34" t="s">
         <v>273</v>
@@ -2861,8 +2918,8 @@
       <c r="C41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="26">
-        <v>9820089688</v>
+      <c r="D41" s="1">
+        <v>8082530463</v>
       </c>
       <c r="E41" s="34" t="s">
         <v>274</v>
@@ -2885,9 +2942,7 @@
         <v>154</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="26">
-        <v>9820089688</v>
-      </c>
+      <c r="D42" s="4"/>
       <c r="E42" s="34" t="s">
         <v>275</v>
       </c>
@@ -2909,8 +2964,8 @@
       <c r="C43" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="26">
-        <v>9820089688</v>
+      <c r="D43" s="1">
+        <v>9892146228</v>
       </c>
       <c r="E43" s="34" t="s">
         <v>276</v>
@@ -2935,8 +2990,8 @@
       <c r="C44" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="26">
-        <v>9820089688</v>
+      <c r="D44" s="1">
+        <v>9869338196</v>
       </c>
       <c r="E44" s="34" t="s">
         <v>277</v>
@@ -2959,8 +3014,8 @@
       <c r="C45" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="26">
-        <v>9820089688</v>
+      <c r="D45" s="1">
+        <v>9819590019</v>
       </c>
       <c r="E45" s="34" t="s">
         <v>239</v>
@@ -2983,8 +3038,8 @@
       <c r="C46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="26">
-        <v>9820089688</v>
+      <c r="D46" s="6">
+        <v>9821138904</v>
       </c>
       <c r="E46" s="34" t="s">
         <v>278</v>
@@ -3007,8 +3062,8 @@
       <c r="C47" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="26">
-        <v>9820089688</v>
+      <c r="D47" s="1">
+        <v>9767172500</v>
       </c>
       <c r="E47" s="34" t="s">
         <v>279</v>
@@ -3033,8 +3088,8 @@
       <c r="C48" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="26">
-        <v>9820089688</v>
+      <c r="D48" s="6">
+        <v>9870079484</v>
       </c>
       <c r="E48" s="34" t="s">
         <v>280</v>
@@ -3059,8 +3114,8 @@
       <c r="C49" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="26">
-        <v>9820089688</v>
+      <c r="D49" s="6">
+        <v>9821211800</v>
       </c>
       <c r="E49" s="34" t="s">
         <v>281</v>
@@ -3085,8 +3140,8 @@
       <c r="C50" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D50" s="26">
-        <v>9820089688</v>
+      <c r="D50" s="1">
+        <v>8655438664</v>
       </c>
       <c r="E50" s="34" t="s">
         <v>282</v>
@@ -3111,8 +3166,8 @@
       <c r="C51" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D51" s="26">
-        <v>9820089688</v>
+      <c r="D51" s="6">
+        <v>9322263691</v>
       </c>
       <c r="E51" s="34" t="s">
         <v>283</v>
@@ -3135,8 +3190,8 @@
       <c r="C52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D52" s="26">
-        <v>9820089688</v>
+      <c r="D52" s="1">
+        <v>9833664559</v>
       </c>
       <c r="E52" s="34" t="s">
         <v>284</v>
@@ -3161,8 +3216,8 @@
       <c r="C53" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="26">
-        <v>9820089688</v>
+      <c r="D53" s="6">
+        <v>9819328305</v>
       </c>
       <c r="E53" s="34" t="s">
         <v>285</v>
@@ -3187,8 +3242,8 @@
       <c r="C54" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="26">
-        <v>9820089688</v>
+      <c r="D54" s="1">
+        <v>9892331557</v>
       </c>
       <c r="E54" s="34" t="s">
         <v>286</v>
@@ -3213,8 +3268,8 @@
       <c r="C55" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D55" s="26">
-        <v>9820089688</v>
+      <c r="D55" s="6">
+        <v>9619454836</v>
       </c>
       <c r="E55" s="34" t="s">
         <v>287</v>
@@ -3237,8 +3292,8 @@
       <c r="C56" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="26">
-        <v>9820089688</v>
+      <c r="D56" s="1">
+        <v>9167429407</v>
       </c>
       <c r="E56" s="34" t="s">
         <v>288</v>
@@ -3263,8 +3318,8 @@
       <c r="C57" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="26">
-        <v>9820089688</v>
+      <c r="D57" s="6">
+        <v>9833801886</v>
       </c>
       <c r="E57" s="34" t="s">
         <v>289</v>
@@ -3287,8 +3342,8 @@
         <v>207</v>
       </c>
       <c r="C58" s="1"/>
-      <c r="D58" s="26">
-        <v>9820089688</v>
+      <c r="D58" s="1">
+        <v>989282815</v>
       </c>
       <c r="E58" s="34" t="s">
         <v>290</v>
@@ -3311,8 +3366,8 @@
         <v>194</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="26">
-        <v>9820089688</v>
+      <c r="D59" s="1">
+        <v>9923215321</v>
       </c>
       <c r="E59" s="34" t="s">
         <v>291</v>
@@ -3337,8 +3392,8 @@
       <c r="C60" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="26">
-        <v>9820089688</v>
+      <c r="D60" s="6">
+        <v>9619198005</v>
       </c>
       <c r="E60" s="34" t="s">
         <v>292</v>
@@ -3359,9 +3414,7 @@
         <v>153</v>
       </c>
       <c r="C61" s="1"/>
-      <c r="D61" s="26">
-        <v>9820089688</v>
-      </c>
+      <c r="D61" s="4"/>
       <c r="E61" s="34" t="s">
         <v>293</v>
       </c>
@@ -3383,8 +3436,8 @@
       <c r="C62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="26">
-        <v>9820089688</v>
+      <c r="D62" s="1">
+        <v>9773377729</v>
       </c>
       <c r="E62" s="34" t="s">
         <v>294</v>
@@ -3409,8 +3462,8 @@
       <c r="C63" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D63" s="26">
-        <v>9820089688</v>
+      <c r="D63" s="1">
+        <v>7208423637</v>
       </c>
       <c r="E63" s="34" t="s">
         <v>295</v>
@@ -3433,8 +3486,8 @@
       <c r="C64" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D64" s="26">
-        <v>9820089688</v>
+      <c r="D64" s="1">
+        <v>9673422368</v>
       </c>
       <c r="E64" s="34" t="s">
         <v>296</v>
@@ -3459,8 +3512,8 @@
       <c r="C65" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="26">
-        <v>9820089688</v>
+      <c r="D65" s="1">
+        <v>9004870439</v>
       </c>
       <c r="E65" s="34" t="s">
         <v>297</v>
@@ -3486,7 +3539,7 @@
         <v>92</v>
       </c>
       <c r="D66" s="6">
-        <v>7045234320</v>
+        <v>9821115781</v>
       </c>
       <c r="E66" s="34" t="s">
         <v>298</v>
@@ -3511,8 +3564,8 @@
       <c r="C67" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D67" s="6">
-        <v>7045234320</v>
+      <c r="D67" s="1">
+        <v>9819499616</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>299</v>
@@ -3538,7 +3591,7 @@
         <v>52</v>
       </c>
       <c r="D68" s="6">
-        <v>7045234320</v>
+        <v>8693883049</v>
       </c>
       <c r="E68" s="34" t="s">
         <v>300</v>
@@ -3562,7 +3615,7 @@
         <v>52</v>
       </c>
       <c r="D69" s="6">
-        <v>7045234320</v>
+        <v>9820064383</v>
       </c>
       <c r="E69" s="34" t="s">
         <v>301</v>
@@ -3585,8 +3638,8 @@
       <c r="C70" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D70" s="6">
-        <v>7045234320</v>
+      <c r="D70" s="1">
+        <v>9867757813</v>
       </c>
       <c r="E70" s="34" t="s">
         <v>302</v>
@@ -3609,8 +3662,8 @@
       <c r="C71" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D71" s="6">
-        <v>7045234320</v>
+      <c r="D71" s="1">
+        <v>9820611901</v>
       </c>
       <c r="E71" s="34" t="s">
         <v>303</v>
@@ -3633,8 +3686,8 @@
       <c r="C72" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D72" s="6">
-        <v>7045234320</v>
+      <c r="D72" s="6" t="s">
+        <v>389</v>
       </c>
       <c r="E72" s="34" t="s">
         <v>304</v>
@@ -3657,8 +3710,8 @@
       <c r="C73" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D73" s="6">
-        <v>7045234320</v>
+      <c r="D73" s="6" t="s">
+        <v>390</v>
       </c>
       <c r="E73" s="34" t="s">
         <v>305</v>
@@ -3682,7 +3735,7 @@
         <v>52</v>
       </c>
       <c r="D74" s="6">
-        <v>7045234320</v>
+        <v>9773311616</v>
       </c>
       <c r="E74" s="34" t="s">
         <v>306</v>
@@ -3707,8 +3760,8 @@
       <c r="C75" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D75" s="6">
-        <v>7045234320</v>
+      <c r="D75" s="1">
+        <v>9820217190</v>
       </c>
       <c r="E75" s="34" t="s">
         <v>307</v>
@@ -3734,7 +3787,7 @@
         <v>39</v>
       </c>
       <c r="D76" s="6">
-        <v>7045234320</v>
+        <v>9167778193</v>
       </c>
       <c r="E76" s="35" t="s">
         <v>308</v>
@@ -3759,8 +3812,8 @@
       <c r="C77" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D77" s="6">
-        <v>7045234320</v>
+      <c r="D77" s="1">
+        <v>9664220457</v>
       </c>
       <c r="E77" s="35" t="s">
         <v>309</v>
@@ -3785,8 +3838,8 @@
       <c r="C78" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D78" s="6">
-        <v>7045234320</v>
+      <c r="D78" s="1">
+        <v>9833931540</v>
       </c>
       <c r="E78" s="35" t="s">
         <v>310</v>
@@ -3811,8 +3864,8 @@
       <c r="C79" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D79" s="6">
-        <v>7045234320</v>
+      <c r="D79" s="1">
+        <v>8796961710</v>
       </c>
       <c r="E79" s="34" t="s">
         <v>311</v>
@@ -3838,7 +3891,7 @@
         <v>52</v>
       </c>
       <c r="D80" s="6">
-        <v>7045234320</v>
+        <v>9004400077</v>
       </c>
       <c r="E80" s="34" t="s">
         <v>312</v>
@@ -3861,8 +3914,8 @@
       <c r="C81" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D81" s="6">
-        <v>7045234320</v>
+      <c r="D81" s="1">
+        <v>9029127775</v>
       </c>
       <c r="E81" s="34" t="s">
         <v>313</v>
@@ -3887,8 +3940,8 @@
       <c r="C82" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D82" s="6">
-        <v>7045234320</v>
+      <c r="D82" s="1">
+        <v>9967958547</v>
       </c>
       <c r="E82" s="34" t="s">
         <v>314</v>
@@ -3914,7 +3967,7 @@
         <v>52</v>
       </c>
       <c r="D83" s="6">
-        <v>7045234320</v>
+        <v>9920149991</v>
       </c>
       <c r="E83" s="34" t="s">
         <v>315</v>
@@ -3938,7 +3991,7 @@
         <v>52</v>
       </c>
       <c r="D84" s="6">
-        <v>7045234320</v>
+        <v>9833744425</v>
       </c>
       <c r="E84" s="34" t="s">
         <v>316</v>
@@ -3961,8 +4014,8 @@
       <c r="C85" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D85" s="6">
-        <v>7045234320</v>
+      <c r="D85" s="1">
+        <v>9820089752</v>
       </c>
       <c r="E85" s="34" t="s">
         <v>317</v>
@@ -3986,7 +4039,7 @@
         <v>52</v>
       </c>
       <c r="D86" s="6">
-        <v>7045234320</v>
+        <v>9323130014</v>
       </c>
       <c r="E86" s="34" t="s">
         <v>318</v>
@@ -4011,8 +4064,8 @@
       <c r="C87" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D87" s="6">
-        <v>7045234320</v>
+      <c r="D87" s="6" t="s">
+        <v>396</v>
       </c>
       <c r="E87" s="34" t="s">
         <v>319</v>
@@ -4038,7 +4091,7 @@
         <v>52</v>
       </c>
       <c r="D88" s="6">
-        <v>7045234320</v>
+        <v>9819993280</v>
       </c>
       <c r="E88" s="34" t="s">
         <v>320</v>
@@ -4062,7 +4115,7 @@
         <v>52</v>
       </c>
       <c r="D89" s="6">
-        <v>7045234320</v>
+        <v>9819860013</v>
       </c>
       <c r="E89" s="34" t="s">
         <v>321</v>
@@ -4087,8 +4140,8 @@
       <c r="C90" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D90" s="6">
-        <v>7045234320</v>
+      <c r="D90" s="1">
+        <v>9699229521</v>
       </c>
       <c r="E90" s="34" t="s">
         <v>322</v>
@@ -4112,7 +4165,7 @@
         <v>39</v>
       </c>
       <c r="D91" s="6">
-        <v>7045234320</v>
+        <v>9920166331</v>
       </c>
       <c r="E91" s="34" t="s">
         <v>323</v>
@@ -4135,8 +4188,8 @@
       <c r="C92" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D92" s="6">
-        <v>7045234320</v>
+      <c r="D92" s="1">
+        <v>9869258741</v>
       </c>
       <c r="E92" s="34" t="s">
         <v>324</v>
@@ -4161,8 +4214,8 @@
       <c r="C93" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D93" s="6">
-        <v>7045234320</v>
+      <c r="D93" s="50">
+        <v>9821947457</v>
       </c>
       <c r="E93" s="34" t="s">
         <v>325</v>
@@ -4188,7 +4241,7 @@
         <v>39</v>
       </c>
       <c r="D94" s="6">
-        <v>7045234320</v>
+        <v>9833584763</v>
       </c>
       <c r="E94" s="34" t="s">
         <v>326</v>
@@ -4211,8 +4264,8 @@
       <c r="C95" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D95" s="6">
-        <v>7045234320</v>
+      <c r="D95" s="1">
+        <v>9221836898</v>
       </c>
       <c r="E95" s="34" t="s">
         <v>327</v>
@@ -4238,7 +4291,7 @@
         <v>4</v>
       </c>
       <c r="D96" s="6">
-        <v>7045234320</v>
+        <v>9819567661</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>328</v>
@@ -4263,8 +4316,8 @@
       <c r="C97" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D97" s="6">
-        <v>7045234320</v>
+      <c r="D97" s="1">
+        <v>9967722931</v>
       </c>
       <c r="E97" s="36" t="s">
         <v>329</v>
@@ -4287,8 +4340,8 @@
         <v>181</v>
       </c>
       <c r="C98" s="1"/>
-      <c r="D98" s="6">
-        <v>7045234320</v>
+      <c r="D98" s="1">
+        <v>9820080309</v>
       </c>
       <c r="E98" s="34" t="s">
         <v>330</v>
@@ -4313,8 +4366,8 @@
       <c r="C99" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D99" s="6">
-        <v>7045234320</v>
+      <c r="D99" s="1">
+        <v>9930367088</v>
       </c>
       <c r="E99" s="34" t="s">
         <v>331</v>
@@ -4340,7 +4393,7 @@
         <v>92</v>
       </c>
       <c r="D100" s="6">
-        <v>7045234320</v>
+        <v>9975451711</v>
       </c>
       <c r="E100" s="34" t="s">
         <v>332</v>
@@ -4365,8 +4418,8 @@
       <c r="C101" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D101" s="6">
-        <v>7045234320</v>
+      <c r="D101" s="1">
+        <v>8983624866</v>
       </c>
       <c r="E101" s="34" t="s">
         <v>333</v>
@@ -4391,8 +4444,8 @@
       <c r="C102" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D102" s="6">
-        <v>7045234320</v>
+      <c r="D102" s="1">
+        <v>9820556824</v>
       </c>
       <c r="E102" s="34"/>
       <c r="F102" s="44"/>
@@ -4413,8 +4466,8 @@
       <c r="C103" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D103" s="6">
-        <v>7045234320</v>
+      <c r="D103" s="6" t="s">
+        <v>391</v>
       </c>
       <c r="E103" s="34" t="s">
         <v>334</v>
@@ -4439,8 +4492,8 @@
       <c r="C104" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D104" s="6">
-        <v>7045234320</v>
+      <c r="D104" s="1">
+        <v>9867761163</v>
       </c>
       <c r="E104" s="34" t="s">
         <v>335</v>
@@ -4465,8 +4518,8 @@
       <c r="C105" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D105" s="6">
-        <v>7045234320</v>
+      <c r="D105" s="1">
+        <v>9821037859</v>
       </c>
       <c r="E105" s="34" t="s">
         <v>336</v>
@@ -4489,8 +4542,8 @@
       <c r="C106" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D106" s="6">
-        <v>7045234320</v>
+      <c r="D106" s="1">
+        <v>9702011541</v>
       </c>
       <c r="E106" s="34" t="s">
         <v>337</v>
@@ -4512,7 +4565,7 @@
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="6">
-        <v>7045234320</v>
+        <v>9820224671</v>
       </c>
       <c r="E107" s="34" t="s">
         <v>338</v>
@@ -4536,7 +4589,7 @@
         <v>121</v>
       </c>
       <c r="D108" s="6">
-        <v>7045234320</v>
+        <v>9702974567</v>
       </c>
       <c r="E108" s="34" t="s">
         <v>339</v>
@@ -4560,7 +4613,7 @@
         <v>52</v>
       </c>
       <c r="D109" s="6">
-        <v>7045234320</v>
+        <v>9820685829</v>
       </c>
       <c r="E109" s="34" t="s">
         <v>340</v>
@@ -4583,8 +4636,8 @@
         <v>208</v>
       </c>
       <c r="C110" s="1"/>
-      <c r="D110" s="6">
-        <v>7045234320</v>
+      <c r="D110" s="1">
+        <v>9769785856</v>
       </c>
       <c r="E110" s="34" t="s">
         <v>341</v>
@@ -4609,8 +4662,8 @@
       <c r="C111" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="6">
-        <v>7045234320</v>
+      <c r="D111" s="1">
+        <v>9820948063</v>
       </c>
       <c r="E111" s="34" t="s">
         <v>234</v>
@@ -4636,7 +4689,7 @@
         <v>52</v>
       </c>
       <c r="D112" s="6">
-        <v>7045234320</v>
+        <v>9975047799</v>
       </c>
       <c r="E112" s="34" t="s">
         <v>342</v>
@@ -4659,8 +4712,8 @@
       <c r="C113" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D113" s="6">
-        <v>7045234320</v>
+      <c r="D113" s="1">
+        <v>9167136048</v>
       </c>
       <c r="E113" s="34" t="s">
         <v>343</v>
@@ -4686,7 +4739,7 @@
         <v>92</v>
       </c>
       <c r="D114" s="6">
-        <v>7045234320</v>
+        <v>9321311122</v>
       </c>
       <c r="E114" s="34" t="s">
         <v>344</v>
@@ -4711,8 +4764,8 @@
       <c r="C115" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D115" s="6">
-        <v>7045234320</v>
+      <c r="D115" s="1">
+        <v>9820921246</v>
       </c>
       <c r="E115" s="34" t="s">
         <v>345</v>
@@ -4737,8 +4790,8 @@
       <c r="C116" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D116" s="6">
-        <v>7045234320</v>
+      <c r="D116" s="6" t="s">
+        <v>392</v>
       </c>
       <c r="E116" s="34" t="s">
         <v>240</v>
@@ -4763,8 +4816,8 @@
       <c r="C117" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D117" s="6">
-        <v>7045234320</v>
+      <c r="D117" s="1">
+        <v>9167768186</v>
       </c>
       <c r="E117" s="34" t="s">
         <v>346</v>
@@ -4790,7 +4843,7 @@
         <v>52</v>
       </c>
       <c r="D118" s="6">
-        <v>7045234320</v>
+        <v>9373609801</v>
       </c>
       <c r="E118" s="34" t="s">
         <v>347</v>
@@ -4814,7 +4867,7 @@
         <v>52</v>
       </c>
       <c r="D119" s="6">
-        <v>7045234320</v>
+        <v>9930041251</v>
       </c>
       <c r="E119" s="34" t="s">
         <v>348</v>
@@ -4840,7 +4893,7 @@
         <v>4</v>
       </c>
       <c r="D120" s="6">
-        <v>7045234320</v>
+        <v>9987903972</v>
       </c>
       <c r="E120" s="34" t="s">
         <v>349</v>
@@ -4865,8 +4918,8 @@
       <c r="C121" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D121" s="6">
-        <v>7045234320</v>
+      <c r="D121" s="1">
+        <v>9833062355</v>
       </c>
       <c r="E121" s="34" t="s">
         <v>350</v>
@@ -4892,7 +4945,7 @@
         <v>52</v>
       </c>
       <c r="D122" s="1">
-        <v>9619410803</v>
+        <v>9867234678</v>
       </c>
       <c r="E122" s="34" t="s">
         <v>351</v>
@@ -4917,8 +4970,8 @@
       <c r="C123" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D123" s="1">
-        <v>9619410803</v>
+      <c r="D123" s="6" t="s">
+        <v>393</v>
       </c>
       <c r="E123" s="34" t="s">
         <v>352</v>
@@ -4942,7 +4995,7 @@
         <v>92</v>
       </c>
       <c r="D124" s="1">
-        <v>9619410803</v>
+        <v>8082500439</v>
       </c>
       <c r="E124" s="34" t="s">
         <v>353</v>
@@ -4967,8 +5020,8 @@
       <c r="C125" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D125" s="1">
-        <v>9619410803</v>
+      <c r="D125" s="6">
+        <v>9773534162</v>
       </c>
       <c r="E125" s="34" t="s">
         <v>354</v>
@@ -4994,7 +5047,7 @@
         <v>4</v>
       </c>
       <c r="D126" s="1">
-        <v>9619410803</v>
+        <v>9819008213</v>
       </c>
       <c r="E126" s="34"/>
       <c r="F126" s="40">
@@ -5017,8 +5070,8 @@
       <c r="C127" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D127" s="1">
-        <v>9619410803</v>
+      <c r="D127" s="6">
+        <v>9967554452</v>
       </c>
       <c r="E127" s="34" t="s">
         <v>355</v>
@@ -5043,8 +5096,8 @@
       <c r="C128" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D128" s="1">
-        <v>9619410803</v>
+      <c r="D128" s="6">
+        <v>9323754718</v>
       </c>
       <c r="E128" s="34" t="s">
         <v>356</v>
@@ -5069,8 +5122,8 @@
       <c r="C129" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D129" s="1">
-        <v>9619410803</v>
+      <c r="D129" s="5">
+        <v>9869504472</v>
       </c>
       <c r="E129" s="34" t="s">
         <v>357</v>
@@ -5093,8 +5146,8 @@
       <c r="C130" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D130" s="1">
-        <v>9619410803</v>
+      <c r="D130" s="6">
+        <v>9869752049</v>
       </c>
       <c r="E130" s="34" t="s">
         <v>358</v>
@@ -5118,7 +5171,7 @@
         <v>121</v>
       </c>
       <c r="D131" s="1">
-        <v>9619410803</v>
+        <v>9004170865</v>
       </c>
       <c r="E131" s="34" t="s">
         <v>359</v>
@@ -5141,8 +5194,8 @@
       <c r="C132" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D132" s="1">
-        <v>9619410803</v>
+      <c r="D132" s="6">
+        <v>9004170865</v>
       </c>
       <c r="E132" s="34"/>
       <c r="F132" s="40">
@@ -5163,8 +5216,8 @@
       <c r="C133" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D133" s="1">
-        <v>9619410803</v>
+      <c r="D133" s="6">
+        <v>9819514290</v>
       </c>
       <c r="E133" s="34" t="s">
         <v>360</v>
@@ -5188,7 +5241,7 @@
         <v>39</v>
       </c>
       <c r="D134" s="1">
-        <v>9619410803</v>
+        <v>9930794227</v>
       </c>
       <c r="E134" s="34" t="s">
         <v>361</v>
@@ -5211,8 +5264,8 @@
       <c r="C135" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D135" s="1">
-        <v>9619410803</v>
+      <c r="D135" s="5">
+        <v>9022946420</v>
       </c>
       <c r="E135" s="34" t="s">
         <v>362</v>
@@ -5238,7 +5291,7 @@
         <v>121</v>
       </c>
       <c r="D136" s="1">
-        <v>9619410803</v>
+        <v>9029879046</v>
       </c>
       <c r="E136" s="34" t="s">
         <v>363</v>
@@ -5263,8 +5316,8 @@
       <c r="C137" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D137" s="1">
-        <v>9619410803</v>
+      <c r="D137" s="5">
+        <v>9619990688</v>
       </c>
       <c r="E137" s="34" t="s">
         <v>364</v>
@@ -5287,8 +5340,8 @@
       <c r="C138" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D138" s="1">
-        <v>9619410803</v>
+      <c r="D138" s="6" t="s">
+        <v>394</v>
       </c>
       <c r="E138" s="34" t="s">
         <v>365</v>
@@ -5312,7 +5365,7 @@
         <v>92</v>
       </c>
       <c r="D139" s="1">
-        <v>9619410803</v>
+        <v>9820250905</v>
       </c>
       <c r="E139" s="34" t="s">
         <v>366</v>
@@ -5337,8 +5390,8 @@
       <c r="C140" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D140" s="1">
-        <v>9619410803</v>
+      <c r="D140" s="6">
+        <v>9619163547</v>
       </c>
       <c r="E140" s="34" t="s">
         <v>367</v>
@@ -5363,8 +5416,8 @@
       <c r="C141" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D141" s="1">
-        <v>9619410803</v>
+      <c r="D141" s="6">
+        <v>9320027236</v>
       </c>
       <c r="E141" s="34" t="s">
         <v>368</v>
@@ -5388,7 +5441,7 @@
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1">
-        <v>9619410803</v>
+        <v>9833870230</v>
       </c>
       <c r="E142" s="34" t="s">
         <v>369</v>
@@ -5414,7 +5467,7 @@
         <v>4</v>
       </c>
       <c r="D143" s="1">
-        <v>9619410803</v>
+        <v>9167181926</v>
       </c>
       <c r="E143" s="34" t="s">
         <v>254</v>
@@ -5438,7 +5491,7 @@
         <v>4</v>
       </c>
       <c r="D144" s="1">
-        <v>9619410803</v>
+        <v>9892953269</v>
       </c>
       <c r="E144" s="34" t="s">
         <v>370</v>
@@ -5464,7 +5517,7 @@
         <v>121</v>
       </c>
       <c r="D145" s="1">
-        <v>9619410803</v>
+        <v>9029548270</v>
       </c>
       <c r="E145" s="34" t="s">
         <v>371</v>
@@ -5490,7 +5543,7 @@
         <v>92</v>
       </c>
       <c r="D146" s="1">
-        <v>9619410803</v>
+        <v>9820258875</v>
       </c>
       <c r="E146" s="34" t="s">
         <v>372</v>
@@ -5513,8 +5566,8 @@
       <c r="C147" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D147" s="1">
-        <v>9619410803</v>
+      <c r="D147" s="6">
+        <v>9869565961</v>
       </c>
       <c r="E147" s="34" t="s">
         <v>373</v>
@@ -5537,8 +5590,8 @@
       <c r="C148" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D148" s="1">
-        <v>9619410803</v>
+      <c r="D148" s="6" t="s">
+        <v>395</v>
       </c>
       <c r="E148" s="34" t="s">
         <v>374</v>
@@ -5563,8 +5616,8 @@
       <c r="C149" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D149" s="1">
-        <v>9619410803</v>
+      <c r="D149" s="50">
+        <v>9702975988</v>
       </c>
       <c r="E149" s="34"/>
       <c r="F149" s="44"/>
@@ -5584,7 +5637,7 @@
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1">
-        <v>9619410803</v>
+        <v>8237281857</v>
       </c>
       <c r="E150" s="34" t="s">
         <v>375</v>
@@ -5609,8 +5662,8 @@
       <c r="C151" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D151" s="1">
-        <v>9619410803</v>
+      <c r="D151" s="51">
+        <v>9967538490</v>
       </c>
       <c r="E151" s="34" t="s">
         <v>376</v>
@@ -5633,8 +5686,8 @@
       <c r="C152" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D152" s="1">
-        <v>9619410803</v>
+      <c r="D152" s="5">
+        <v>9167264495</v>
       </c>
       <c r="E152" s="34" t="s">
         <v>377</v>
@@ -5658,7 +5711,7 @@
         <v>92</v>
       </c>
       <c r="D153" s="1">
-        <v>9619410803</v>
+        <v>9167264495</v>
       </c>
       <c r="E153" s="34" t="s">
         <v>378</v>
@@ -5681,8 +5734,8 @@
       <c r="C154" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D154" s="1">
-        <v>9619410803</v>
+      <c r="D154" s="6">
+        <v>9869110162</v>
       </c>
       <c r="E154" s="34" t="s">
         <v>379</v>
@@ -5707,8 +5760,8 @@
       <c r="C155" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D155" s="1">
-        <v>9619410803</v>
+      <c r="D155" s="6">
+        <v>9987368383</v>
       </c>
       <c r="E155" s="34" t="s">
         <v>380</v>
@@ -5731,8 +5784,8 @@
       <c r="C156" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D156" s="1">
-        <v>9619410803</v>
+      <c r="D156" s="5">
+        <v>9769383381</v>
       </c>
       <c r="E156" s="34" t="s">
         <v>381</v>
@@ -5755,8 +5808,8 @@
       <c r="C157" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D157" s="1">
-        <v>9619410803</v>
+      <c r="D157" s="22">
+        <v>9820146448</v>
       </c>
       <c r="E157" s="36" t="s">
         <v>382</v>
@@ -5780,7 +5833,7 @@
         <v>52</v>
       </c>
       <c r="D158" s="1">
-        <v>9619410803</v>
+        <v>7208108017</v>
       </c>
       <c r="E158" s="34" t="s">
         <v>383</v>
@@ -5805,8 +5858,8 @@
       <c r="C159" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D159" s="1">
-        <v>9619410803</v>
+      <c r="D159" s="5">
+        <v>9833370596</v>
       </c>
       <c r="E159" s="34"/>
       <c r="F159" s="40">
@@ -5829,8 +5882,8 @@
       <c r="C160" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D160" s="1">
-        <v>9619410803</v>
+      <c r="D160" s="6">
+        <v>9892096803</v>
       </c>
       <c r="E160" s="34" t="s">
         <v>384</v>
@@ -5854,7 +5907,7 @@
         <v>121</v>
       </c>
       <c r="D161" s="1">
-        <v>9619410803</v>
+        <v>9892096803</v>
       </c>
       <c r="E161" s="34" t="s">
         <v>385</v>
@@ -5877,8 +5930,8 @@
       <c r="C162" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D162" s="1">
-        <v>9619410803</v>
+      <c r="D162" s="6">
+        <v>9819614795</v>
       </c>
       <c r="E162" s="34" t="s">
         <v>281</v>

</xml_diff>